<commit_message>
add: CRUD for lecturer
</commit_message>
<xml_diff>
--- a/public/template/template_import_users.xlsx
+++ b/public/template/template_import_users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prian\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\artilearning\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608FD545-4306-43C3-8502-7763A293A51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC136BC5-44C1-4C0E-A902-5EDA6FEFBE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FD4805BB-777A-4EF5-9294-F9AAC11FFF25}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>